<commit_message>
Add changes - tokenizacion
</commit_message>
<xml_diff>
--- a/data/input/Canciones_Colombianas_1945_2023.xlsx
+++ b/data/input/Canciones_Colombianas_1945_2023.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccca1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ccca1\Documents\Git\AI-university_javeriana-nlp-taller_ley_zipf\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE042028-1D35-4363-93A3-13AD639B048A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68951422-E025-411F-9FF9-537E5C91E015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="248">
   <si>
     <t>La loca Margarita</t>
   </si>
@@ -178,27 +191,15 @@
     <t>Salsa</t>
   </si>
   <si>
-    <t>Balada romántica</t>
-  </si>
-  <si>
     <t>Joropo</t>
   </si>
   <si>
-    <t>Balada pop</t>
-  </si>
-  <si>
     <t>Pop</t>
   </si>
   <si>
-    <t>Vallenato-pop</t>
-  </si>
-  <si>
     <t>Reguetón</t>
   </si>
   <si>
-    <t>Reguetón-pop</t>
-  </si>
-  <si>
     <t>Rafael Godoy (Garzón y Collazos)</t>
   </si>
   <si>
@@ -238,21 +239,9 @@
     <t>Isadora (Fernanda Bustos)</t>
   </si>
   <si>
-    <t>Cumbia tropical</t>
-  </si>
-  <si>
-    <t>Rock en español</t>
-  </si>
-  <si>
-    <t>Vallenato fusión</t>
-  </si>
-  <si>
     <t>Shakira (ft. Freshlyground)</t>
   </si>
   <si>
-    <t>Pop-vallenato</t>
-  </si>
-  <si>
     <t>J Balvin (ft. Farruko)</t>
   </si>
   <si>
@@ -467,75 +456,6 @@
   </si>
   <si>
     <t>genero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porro </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vallenato </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Merecumbé </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rumba criolla </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Currulao </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nueva ola </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Balada </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bolero </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carranga </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pop latino </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jazz-folk </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tropipop </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pop-rock </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rock </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pop rock </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salsa </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pop </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hip-hop </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electro-cumbia </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electro-folk </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Swing </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reguetón </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reguetón-pop </t>
   </si>
   <si>
     <t>letra</t>
@@ -3992,6 +3912,42 @@
 Quiero volver a enamorarte de nuevo
 Todos los días, como si fuera el primero</t>
   </si>
+  <si>
+    <t>Balada</t>
+  </si>
+  <si>
+    <t>Merecumbé</t>
+  </si>
+  <si>
+    <t>Currulao</t>
+  </si>
+  <si>
+    <t>Nueva ola</t>
+  </si>
+  <si>
+    <t>Bolero</t>
+  </si>
+  <si>
+    <t>Carranga</t>
+  </si>
+  <si>
+    <t>Jazz-folk</t>
+  </si>
+  <si>
+    <t>Tropipop</t>
+  </si>
+  <si>
+    <t>Hip-hop</t>
+  </si>
+  <si>
+    <t>Electro-cumbia</t>
+  </si>
+  <si>
+    <t>Electro-folk</t>
+  </si>
+  <si>
+    <t>Swing</t>
+  </si>
 </sst>
 </file>
 
@@ -4053,7 +4009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4064,13 +4020,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4078,7 +4030,21 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4102,6 +4068,20 @@
       <font>
         <b val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -4132,20 +4112,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4159,19 +4125,26 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1CFA7A68-18DE-4418-8E14-E8D9AC5EDDBF}" name="Tabla1" displayName="Tabla1" ref="A1:E78" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="3" tableBorderDxfId="4">
-  <autoFilter ref="A1:E78" xr:uid="{1CFA7A68-18DE-4418-8E14-E8D9AC5EDDBF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1CFA7A68-18DE-4418-8E14-E8D9AC5EDDBF}" name="Tabla1" displayName="Tabla1" ref="A1:E78" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="A1:E78" xr:uid="{1CFA7A68-18DE-4418-8E14-E8D9AC5EDDBF}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Balada pop"/>
+        <filter val="Pop"/>
+        <filter val="Pop latino"/>
+        <filter val="Pop rock"/>
+        <filter val="Pop-rock"/>
+        <filter val="Tropipop"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FA10AC8D-888B-45D2-9BD7-C21D262F3FD9}" name="year" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{38DED43E-0CAD-4270-809C-2635E9FD8389}" name="song" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FA10AC8D-888B-45D2-9BD7-C21D262F3FD9}" name="year" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{38DED43E-0CAD-4270-809C-2635E9FD8389}" name="song" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{BDA1D8B5-9491-4F89-BD68-1286C2E00AB3}" name="autor"/>
     <tableColumn id="3" xr3:uid="{D820AFC3-06DA-45EF-B8F0-66DF294195EB}" name="genero"/>
-    <tableColumn id="8" xr3:uid="{6E0137B3-00D3-4003-ADA2-9F97EADF76D6}" name="letra"/>
+    <tableColumn id="8" xr3:uid="{6E0137B3-00D3-4003-ADA2-9F97EADF76D6}" name="letra" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4466,14 +4439,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="43.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="43.42578125" customWidth="1"/>
     <col min="3" max="3" width="58" customWidth="1"/>
     <col min="4" max="4" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
@@ -4481,60 +4453,60 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1945</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>79</v>
+      <c r="B2" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+        <v>45</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>1946</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>80</v>
+      <c r="B3" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="E3" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>1947</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -4543,67 +4515,67 @@
       <c r="D4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="E4" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>1948</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>178</v>
+      <c r="B5" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="E5" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>1949</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>81</v>
+      <c r="B6" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="E6" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>1950</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>82</v>
+      <c r="B7" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+        <v>52</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>1951</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>83</v>
+      <c r="B8" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
@@ -4611,50 +4583,50 @@
       <c r="D8" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="E8" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>1952</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>84</v>
+      <c r="B9" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+        <v>49</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>1953</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>85</v>
+      <c r="B10" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+        <v>45</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>1954</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>86</v>
+      <c r="B11" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>7</v>
@@ -4662,33 +4634,33 @@
       <c r="D11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="E11" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>1955</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>87</v>
+      <c r="B12" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+        <v>237</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>1956</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>88</v>
+      <c r="B13" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>9</v>
@@ -4696,84 +4668,84 @@
       <c r="D13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="E13" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>1957</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>89</v>
+      <c r="B14" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+        <v>47</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>1959</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>90</v>
+      <c r="B15" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="E15" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>1960</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>91</v>
+      <c r="B16" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="E16" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>1961</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>92</v>
+      <c r="B17" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="E17" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>1962</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>93</v>
+      <c r="B18" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>10</v>
@@ -4781,50 +4753,50 @@
       <c r="D18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="E18" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>1963</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>94</v>
+      <c r="B19" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="E19" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>1964</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>95</v>
+      <c r="B20" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+        <v>238</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>1965</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>96</v>
+      <c r="B21" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>4</v>
@@ -4832,135 +4804,135 @@
       <c r="D21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="E21" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>1966</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>97</v>
+      <c r="B22" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+        <v>239</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>1967</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>91</v>
+      <c r="B23" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="E23" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>1968</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>98</v>
+      <c r="B24" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+        <v>49</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>1969</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>99</v>
+      <c r="B25" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+        <v>238</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>1970</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>100</v>
+      <c r="B26" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+        <v>236</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
         <v>1971</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>101</v>
+      <c r="B27" s="3" t="s">
+        <v>93</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="E27" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>1972</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>102</v>
+      <c r="B28" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+        <v>236</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>1973</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>103</v>
+      <c r="B29" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>16</v>
@@ -4968,152 +4940,152 @@
       <c r="D29" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="E29" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
         <v>1974</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>104</v>
+      <c r="B30" s="3" t="s">
+        <v>96</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="E30" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>1975</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>105</v>
+      <c r="B31" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+      <c r="E31" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
         <v>1976</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>106</v>
+      <c r="B32" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+      <c r="E32" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
         <v>1977</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>107</v>
+      <c r="B33" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+        <v>236</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
         <v>1978</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>108</v>
+      <c r="B34" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
+        <v>240</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
         <v>1979</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>109</v>
+      <c r="B35" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
+        <v>50</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
         <v>1980</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>110</v>
+      <c r="B36" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+        <v>241</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
         <v>1981</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>111</v>
+      <c r="B37" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+        <v>52</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
         <v>1982</v>
       </c>
-      <c r="B38" s="5" t="s">
-        <v>112</v>
+      <c r="B38" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>21</v>
@@ -5121,16 +5093,16 @@
       <c r="D38" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E38" s="7" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+      <c r="E38" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
         <v>1983</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>113</v>
+      <c r="B39" s="3" t="s">
+        <v>105</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>22</v>
@@ -5138,16 +5110,16 @@
       <c r="D39" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+      <c r="E39" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
         <v>1984</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>114</v>
+      <c r="B40" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>23</v>
@@ -5155,33 +5127,33 @@
       <c r="D40" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="7" t="s">
-        <v>213</v>
+      <c r="E40" s="5" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+      <c r="A41" s="3">
         <v>1985</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>214</v>
+      <c r="B41" s="3" t="s">
+        <v>183</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+        <v>236</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
         <v>1986</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>115</v>
+      <c r="B42" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>25</v>
@@ -5189,67 +5161,67 @@
       <c r="D42" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E42" s="7" t="s">
-        <v>216</v>
+      <c r="E42" s="5" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
+      <c r="A43" s="3">
         <v>1987</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>116</v>
+      <c r="B43" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
+        <v>236</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
         <v>1988</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>117</v>
+      <c r="B44" s="3" t="s">
+        <v>109</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
+        <v>205</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
         <v>1989</v>
       </c>
       <c r="B45" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="C45" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+        <v>236</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
         <v>1990</v>
       </c>
-      <c r="B46" s="5" t="s">
-        <v>118</v>
+      <c r="B46" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>23</v>
@@ -5257,50 +5229,50 @@
       <c r="D46" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="7" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
+      <c r="E46" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
         <v>1991</v>
       </c>
       <c r="B47" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="C47" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5">
+      <c r="E47" s="5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
         <v>1993</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>119</v>
+      <c r="B48" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="5">
+        <v>49</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
         <v>1994</v>
       </c>
-      <c r="B49" s="5" t="s">
-        <v>120</v>
+      <c r="B49" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>29</v>
@@ -5308,501 +5280,501 @@
       <c r="D49" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>227</v>
+      <c r="E49" s="5" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
+      <c r="A50" s="3">
         <v>1995</v>
       </c>
-      <c r="B50" s="5" t="s">
-        <v>121</v>
+      <c r="B50" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5">
+        <v>53</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
         <v>1996</v>
       </c>
       <c r="B51" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="C51" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>229</v>
+        <v>242</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="5">
+      <c r="A52" s="3">
         <v>1997</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>122</v>
+      <c r="B52" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5">
+        <v>243</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
         <v>1998</v>
       </c>
       <c r="B53" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="C53" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>233</v>
+        <v>205</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="5">
+      <c r="A54" s="3">
         <v>1999</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>123</v>
+      <c r="B54" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5">
+        <v>53</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
         <v>2000</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>124</v>
+      <c r="B55" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E55" s="7" t="s">
-        <v>238</v>
+        <v>205</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="5">
+      <c r="A56" s="3">
         <v>2001</v>
       </c>
-      <c r="B56" s="5" t="s">
-        <v>125</v>
+      <c r="B56" s="3" t="s">
+        <v>117</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
+        <v>53</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
         <v>2002</v>
       </c>
-      <c r="B57" s="5" t="s">
-        <v>126</v>
+      <c r="B57" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="5">
+        <v>205</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
         <v>2004</v>
       </c>
-      <c r="B58" s="5" t="s">
-        <v>127</v>
+      <c r="B58" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>241</v>
+        <v>51</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="5">
+      <c r="A59" s="3">
         <v>2005</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>128</v>
+      <c r="B59" s="3" t="s">
+        <v>120</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
+        <v>53</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
         <v>2007</v>
       </c>
-      <c r="B60" s="5" t="s">
-        <v>129</v>
+      <c r="B60" s="3" t="s">
+        <v>121</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
+        <v>244</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
         <v>2008</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>130</v>
+      <c r="B61" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>35</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="5">
+        <v>245</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
         <v>2009</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>131</v>
+      <c r="B62" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>245</v>
+        <v>246</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
+      <c r="A63" s="3">
         <v>2010</v>
       </c>
-      <c r="B63" s="5" t="s">
-        <v>246</v>
+      <c r="B63" s="3" t="s">
+        <v>215</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="5">
+        <v>53</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
         <v>2011</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>132</v>
+      <c r="B64" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
+        <v>244</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
         <v>2012</v>
       </c>
-      <c r="B65" s="5" t="s">
-        <v>133</v>
+      <c r="B65" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="5">
+        <v>247</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
         <v>2013</v>
       </c>
-      <c r="B66" s="5" t="s">
-        <v>134</v>
+      <c r="B66" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>28</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E66" s="7" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="5">
+        <v>49</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
         <v>2014</v>
       </c>
-      <c r="B67" s="5" t="s">
-        <v>135</v>
+      <c r="B67" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="5">
+        <v>54</v>
+      </c>
+      <c r="E67" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
         <v>2015</v>
       </c>
-      <c r="B68" s="5" t="s">
-        <v>136</v>
+      <c r="B68" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="5">
+        <v>54</v>
+      </c>
+      <c r="E68" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
         <v>2016</v>
       </c>
-      <c r="B69" s="5" t="s">
-        <v>137</v>
+      <c r="B69" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="5">
+        <v>49</v>
+      </c>
+      <c r="E69" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
         <v>2017</v>
       </c>
-      <c r="B70" s="5" t="s">
-        <v>138</v>
+      <c r="B70" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="5">
+        <v>54</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
         <v>2018</v>
       </c>
-      <c r="B71" s="5" t="s">
-        <v>139</v>
+      <c r="B71" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="5">
+        <v>54</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
         <v>2019</v>
       </c>
-      <c r="B72" s="5" t="s">
-        <v>140</v>
+      <c r="B72" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="5">
+        <v>54</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
         <v>2020</v>
       </c>
-      <c r="B73" s="5" t="s">
-        <v>141</v>
+      <c r="B73" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>43</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E73" s="7" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="5">
+        <v>54</v>
+      </c>
+      <c r="E73" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
         <v>2021</v>
       </c>
-      <c r="B74" s="5" t="s">
-        <v>142</v>
+      <c r="B74" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E74" s="7" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="5">
+        <v>54</v>
+      </c>
+      <c r="E74" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
         <v>2022</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>143</v>
+      <c r="B75" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>42</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="5">
+        <v>54</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
         <v>2023</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>144</v>
+      <c r="B76" s="3" t="s">
+        <v>136</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>44</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="6">
+        <v>54</v>
+      </c>
+      <c r="E76" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>2024</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>261</v>
+      <c r="B77" s="3" t="s">
+        <v>230</v>
       </c>
       <c r="C77" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>262</v>
+        <v>54</v>
+      </c>
+      <c r="E77" s="5" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="6">
+      <c r="A78">
         <v>2025</v>
       </c>
-      <c r="B78" s="5" t="s">
-        <v>264</v>
+      <c r="B78" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="C78" t="s">
-        <v>265</v>
+        <v>234</v>
       </c>
       <c r="D78" t="s">
-        <v>55</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>266</v>
+        <v>53</v>
+      </c>
+      <c r="E78" s="5" t="s">
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>